<commit_message>
nuts2 regions are basically finished
</commit_message>
<xml_diff>
--- a/input/general/Abbreviations.xlsx
+++ b/input/general/Abbreviations.xlsx
@@ -1355,7 +1355,7 @@
     <t xml:space="preserve">Griechenland</t>
   </si>
   <si>
-    <t xml:space="preserve">GR</t>
+    <t xml:space="preserve">EL</t>
   </si>
   <si>
     <t xml:space="preserve">GRC</t>
@@ -3407,7 +3407,7 @@
     <t xml:space="preserve">Vereinigtes Königreich</t>
   </si>
   <si>
-    <t xml:space="preserve">GB</t>
+    <t xml:space="preserve">UK</t>
   </si>
   <si>
     <t xml:space="preserve">GBR</t>
@@ -3626,59 +3626,13 @@
     <t xml:space="preserve">[1]</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">English names, abbreviations, region etc. adapted from</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/lukes/ISO-3166-Countries-with-Regional-Codes/blob/master/all/all.csv</t>
-    </r>
+    <t xml:space="preserve">English names, abbreviations, region etc. adapted from https://github.com/lukes/ISO-3166-Countries-with-Regional-Codes/blob/master/all/all.csv</t>
   </si>
   <si>
     <t xml:space="preserve">[2]</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">German translations adapted from </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://stefangabos.github.io/world_countries/</t>
-    </r>
+    <t xml:space="preserve">German translations adapted from https://stefangabos.github.io/world_countries/</t>
   </si>
 </sst>
 </file>
@@ -3688,7 +3642,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3710,12 +3664,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3760,7 +3708,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3769,7 +3717,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3792,8 +3744,8 @@
   </sheetPr>
   <dimension ref="A1:L250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A223" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C235" activeCellId="0" sqref="C235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6866,7 +6818,7 @@
       <c r="B88" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="2" t="s">
         <v>444</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -12475,36 +12427,36 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>1199</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>1200</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>1201</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>1202</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>1203</v>
       </c>
     </row>
@@ -12513,7 +12465,7 @@
     <mergeCell ref="B4:O4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://stefangabos.github.io/world_countries/"/>
+    <hyperlink ref="B5" r:id="rId1" display="German translations adapted from https://stefangabos.github.io/world_countries/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
specific consumption timeseries now are correctly calculated. But the coefficients are not the same as the reference
</commit_message>
<xml_diff>
--- a/input/general/Abbreviations.xlsx
+++ b/input/general/Abbreviations.xlsx
@@ -308,7 +308,7 @@
     <t xml:space="preserve">Austria</t>
   </si>
   <si>
-    <t xml:space="preserve">Österreich</t>
+    <t xml:space="preserve">Oesterreich</t>
   </si>
   <si>
     <t xml:space="preserve">AT</t>
@@ -983,7 +983,7 @@
     <t xml:space="preserve">Denmark</t>
   </si>
   <si>
-    <t xml:space="preserve">Dänemark</t>
+    <t xml:space="preserve">Daenemark</t>
   </si>
   <si>
     <t xml:space="preserve">DK</t>
@@ -2672,7 +2672,7 @@
     <t xml:space="preserve">Romania</t>
   </si>
   <si>
-    <t xml:space="preserve">Rumänien</t>
+    <t xml:space="preserve">Rumaenien</t>
   </si>
   <si>
     <t xml:space="preserve">RO</t>
@@ -3404,7 +3404,7 @@
     <t xml:space="preserve">United Kingdom</t>
   </si>
   <si>
-    <t xml:space="preserve">Vereinigtes Königreich</t>
+    <t xml:space="preserve">Vereinigtes Koenigreich</t>
   </si>
   <si>
     <t xml:space="preserve">UK</t>
@@ -3744,8 +3744,8 @@
   </sheetPr>
   <dimension ref="A1:L250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A223" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C235" activeCellId="0" sqref="C235"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A167" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B184" activeCellId="0" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>